<commit_message>
Still iterating through things twice
</commit_message>
<xml_diff>
--- a/Fitch Scheduling Machine/ScheduleA.xlsx
+++ b/Fitch Scheduling Machine/ScheduleA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>DAY</t>
   </si>
@@ -35,352 +35,22 @@
     <t>P1</t>
   </si>
   <si>
-    <t>Out Ed A</t>
-  </si>
-  <si>
-    <t>Phys Ed C</t>
-  </si>
-  <si>
-    <t>Phys Ed A</t>
-  </si>
-  <si>
-    <t>Phys Ed WOTP AM</t>
-  </si>
-  <si>
-    <t>Phys Ed NV</t>
-  </si>
-  <si>
-    <t>Out Ed B</t>
-  </si>
-  <si>
-    <t>Phys Ed D</t>
-  </si>
-  <si>
-    <t>Phys Ed B</t>
-  </si>
-  <si>
-    <t>Work1 WOTP PM</t>
-  </si>
-  <si>
-    <t>French A</t>
-  </si>
-  <si>
     <t/>
-  </si>
-  <si>
-    <t>French C</t>
-  </si>
-  <si>
-    <t>Math B</t>
-  </si>
-  <si>
-    <t>Math D</t>
-  </si>
-  <si>
-    <t>English C</t>
-  </si>
-  <si>
-    <t>French E</t>
-  </si>
-  <si>
-    <t>English E</t>
-  </si>
-  <si>
-    <t>Math E</t>
-  </si>
-  <si>
-    <t>English F</t>
-  </si>
-  <si>
-    <t>French F</t>
-  </si>
-  <si>
-    <t>CCQ G</t>
-  </si>
-  <si>
-    <t>Math G</t>
-  </si>
-  <si>
-    <t>English G</t>
-  </si>
-  <si>
-    <t>CCQ F</t>
-  </si>
-  <si>
-    <t>English NV</t>
-  </si>
-  <si>
-    <t>French G</t>
-  </si>
-  <si>
-    <t>French JS</t>
-  </si>
-  <si>
-    <t>French NV</t>
-  </si>
-  <si>
-    <t>English WOTP AM</t>
-  </si>
-  <si>
-    <t>Science JS</t>
   </si>
   <si>
     <t>P2</t>
   </si>
   <si>
-    <t>Out Ed C</t>
-  </si>
-  <si>
-    <t>Out Ed Ex A</t>
-  </si>
-  <si>
-    <t>Out Ed Ex C</t>
-  </si>
-  <si>
-    <t>Out Ed Ex E</t>
-  </si>
-  <si>
-    <t>Phys Ed JS</t>
-  </si>
-  <si>
-    <t>Out Ed D</t>
-  </si>
-  <si>
-    <t>Out Ed Ex B</t>
-  </si>
-  <si>
-    <t>Out Ed Ex D</t>
-  </si>
-  <si>
-    <t>Out Ed Ex F</t>
-  </si>
-  <si>
-    <t>Work2 WOTP PM</t>
-  </si>
-  <si>
-    <t>Out Ed Ex G</t>
-  </si>
-  <si>
-    <t>Math A</t>
-  </si>
-  <si>
-    <t>French B</t>
-  </si>
-  <si>
-    <t>Science F</t>
-  </si>
-  <si>
-    <t>Science C</t>
-  </si>
-  <si>
-    <t>Science G</t>
-  </si>
-  <si>
-    <t>English D</t>
-  </si>
-  <si>
-    <t>Tech F</t>
-  </si>
-  <si>
-    <t>Tech G</t>
-  </si>
-  <si>
-    <t>English JS</t>
-  </si>
-  <si>
-    <t>English2 WOTP AM</t>
-  </si>
-  <si>
-    <t>Math WOTP AM</t>
-  </si>
-  <si>
     <t>P3</t>
-  </si>
-  <si>
-    <t>Out Ed E</t>
-  </si>
-  <si>
-    <t>Out Ed F</t>
-  </si>
-  <si>
-    <t>Out Ed G</t>
-  </si>
-  <si>
-    <t>Work3 WOTP PM</t>
-  </si>
-  <si>
-    <t>CCQ Sc4Boys F</t>
-  </si>
-  <si>
-    <t>Math C</t>
-  </si>
-  <si>
-    <t>CCQ Sc4Boys G</t>
-  </si>
-  <si>
-    <t>French D</t>
-  </si>
-  <si>
-    <t>English A</t>
-  </si>
-  <si>
-    <t>Science E</t>
-  </si>
-  <si>
-    <t>English B</t>
-  </si>
-  <si>
-    <t>Math F</t>
-  </si>
-  <si>
-    <t>Science D</t>
-  </si>
-  <si>
-    <t>Science NV</t>
-  </si>
-  <si>
-    <t>Tech D</t>
-  </si>
-  <si>
-    <t>History JS</t>
-  </si>
-  <si>
-    <t>Job Market WOTP AM</t>
-  </si>
-  <si>
-    <t>English WOTP PM</t>
-  </si>
-  <si>
-    <t>Math WOTP PM</t>
   </si>
   <si>
     <t>P4</t>
   </si>
   <si>
-    <t>Phys Ed E</t>
-  </si>
-  <si>
-    <t>Work3 WOTP AM</t>
-  </si>
-  <si>
-    <t>Science A</t>
-  </si>
-  <si>
-    <t>Phys Ed F</t>
-  </si>
-  <si>
-    <t>Science B</t>
-  </si>
-  <si>
-    <t>Phys Ed G</t>
-  </si>
-  <si>
-    <t>History NV</t>
-  </si>
-  <si>
-    <t>CCQ NV</t>
-  </si>
-  <si>
-    <t>Math NV</t>
-  </si>
-  <si>
-    <t>French WOTP AM</t>
-  </si>
-  <si>
-    <t>French WOTP PM</t>
-  </si>
-  <si>
     <t>P5</t>
   </si>
   <si>
-    <t>Phys Ed WOTP PM</t>
-  </si>
-  <si>
-    <t>Work2 WOTP AM</t>
-  </si>
-  <si>
-    <t>History C</t>
-  </si>
-  <si>
-    <t>CCQ D</t>
-  </si>
-  <si>
-    <t>CCQ C</t>
-  </si>
-  <si>
-    <t>History D</t>
-  </si>
-  <si>
-    <t>CW D</t>
-  </si>
-  <si>
-    <t>History F</t>
-  </si>
-  <si>
-    <t>Art E</t>
-  </si>
-  <si>
-    <t>History G</t>
-  </si>
-  <si>
-    <t>Music F</t>
-  </si>
-  <si>
-    <t>CW F</t>
-  </si>
-  <si>
-    <t>Music G</t>
-  </si>
-  <si>
-    <t>CW G</t>
-  </si>
-  <si>
-    <t>Art JS</t>
-  </si>
-  <si>
-    <t>CCQ JS</t>
-  </si>
-  <si>
     <t>P6</t>
-  </si>
-  <si>
-    <t>Work1 WOTP AM</t>
-  </si>
-  <si>
-    <t>CCQ A</t>
-  </si>
-  <si>
-    <t>History B</t>
-  </si>
-  <si>
-    <t>History A</t>
-  </si>
-  <si>
-    <t>Art C</t>
-  </si>
-  <si>
-    <t>CCQ B</t>
-  </si>
-  <si>
-    <t>Music D</t>
-  </si>
-  <si>
-    <t>History E</t>
-  </si>
-  <si>
-    <t>Out Ed NV</t>
-  </si>
-  <si>
-    <t>Art NV</t>
-  </si>
-  <si>
-    <t>Math JS</t>
-  </si>
-  <si>
-    <t>English2 WOTP PM</t>
-  </si>
-  <si>
-    <t>Job Market WOTP PM</t>
   </si>
 </sst>
 </file>
@@ -558,340 +228,340 @@
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2"/>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2"/>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2"/>
       <c r="C6" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2"/>
       <c r="C7" s="5" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2"/>
       <c r="C8" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2"/>
       <c r="C9" s="5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2"/>
       <c r="C10" s="5" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2"/>
       <c r="C11" s="5" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2"/>
       <c r="C12" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2"/>
       <c r="C13" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2"/>
       <c r="C14" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2"/>
       <c r="C15" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2"/>
       <c r="C16" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2"/>
       <c r="C17" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2"/>
       <c r="C18" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2"/>
       <c r="C19" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2"/>
       <c r="C20" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3"/>
       <c r="C21" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="22">
@@ -903,346 +573,346 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>37</v>
+        <v>8</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2"/>
       <c r="C24" s="5" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2"/>
       <c r="C25" s="5" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2"/>
       <c r="C26" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2"/>
       <c r="C27" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2"/>
       <c r="C28" s="5" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2"/>
       <c r="C29" s="5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2"/>
       <c r="C30" s="5" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2"/>
       <c r="C31" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2"/>
       <c r="C32" s="5" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2"/>
       <c r="C33" s="5" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2"/>
       <c r="C34" s="5" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2"/>
       <c r="C35" s="5" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2"/>
       <c r="C36" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2"/>
       <c r="C37" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2"/>
       <c r="C38" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F38" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2"/>
       <c r="C39" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2"/>
       <c r="C40" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3"/>
       <c r="C41" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="42">
@@ -1254,346 +924,346 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>60</v>
+        <v>9</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2"/>
       <c r="C44" s="5" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2"/>
       <c r="C45" s="5" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2"/>
       <c r="C46" s="5" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2"/>
       <c r="C47" s="5" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2"/>
       <c r="C48" s="5" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2"/>
       <c r="C49" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2"/>
       <c r="C50" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2"/>
       <c r="C51" s="5" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2"/>
       <c r="C52" s="5" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2"/>
       <c r="C53" s="5" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2"/>
       <c r="C54" s="5" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2"/>
       <c r="C55" s="5" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2"/>
       <c r="C56" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2"/>
       <c r="C57" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2"/>
       <c r="C58" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2"/>
       <c r="C59" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2"/>
       <c r="C60" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3"/>
       <c r="C61" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="62">
@@ -1605,19 +1275,19 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>80</v>
+        <v>10</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>7</v>
@@ -1626,325 +1296,325 @@
     <row r="64">
       <c r="A64" s="2"/>
       <c r="C64" s="5" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2"/>
       <c r="C65" s="5" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2"/>
       <c r="C66" s="5" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2"/>
       <c r="C67" s="5" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2"/>
       <c r="C68" s="5" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2"/>
       <c r="C69" s="5" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2"/>
       <c r="C70" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>88</v>
+        <v>7</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2"/>
       <c r="C71" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E71" s="5" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2"/>
       <c r="C72" s="5" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>90</v>
+        <v>7</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2"/>
       <c r="C73" s="5" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2"/>
       <c r="C74" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2"/>
       <c r="C75" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2"/>
       <c r="C76" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2"/>
       <c r="C77" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2"/>
       <c r="C78" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2"/>
       <c r="C79" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2"/>
       <c r="C80" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3"/>
       <c r="C81" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="82">
@@ -1956,346 +1626,346 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>92</v>
+        <v>11</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2"/>
       <c r="C84" s="5" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2"/>
       <c r="C85" s="5" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2"/>
       <c r="C86" s="5" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2"/>
       <c r="C87" s="5" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2"/>
       <c r="C88" s="5" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>54</v>
+        <v>7</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2"/>
       <c r="C89" s="5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2"/>
       <c r="C90" s="5" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2"/>
       <c r="C91" s="5" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>105</v>
+        <v>7</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2"/>
       <c r="C92" s="5" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2"/>
       <c r="C93" s="5" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2"/>
       <c r="C94" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2"/>
       <c r="C95" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2"/>
       <c r="C96" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2"/>
       <c r="C97" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2"/>
       <c r="C98" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2"/>
       <c r="C99" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2"/>
       <c r="C100" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3"/>
       <c r="C101" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="102">
@@ -2307,346 +1977,346 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>109</v>
+        <v>12</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2"/>
       <c r="C104" s="5" t="s">
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2"/>
       <c r="C105" s="5" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2"/>
       <c r="C106" s="5" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2"/>
       <c r="C107" s="5" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>115</v>
+        <v>7</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2"/>
       <c r="C108" s="5" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>115</v>
+        <v>7</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2"/>
       <c r="C109" s="5" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2"/>
       <c r="C110" s="5" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2"/>
       <c r="C111" s="5" t="s">
-        <v>105</v>
+        <v>7</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2"/>
       <c r="C112" s="5" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>119</v>
+        <v>7</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2"/>
       <c r="C113" s="5" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2"/>
       <c r="C114" s="5" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2"/>
       <c r="C115" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2"/>
       <c r="C116" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2"/>
       <c r="C117" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2"/>
       <c r="C118" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2"/>
       <c r="C119" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2"/>
       <c r="C120" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="3"/>
       <c r="C121" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Oct 1 Update A
</commit_message>
<xml_diff>
--- a/Fitch Scheduling Machine/ScheduleA.xlsx
+++ b/Fitch Scheduling Machine/ScheduleA.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
     <t>DAY</t>
   </si>
@@ -35,373 +35,337 @@
     <t>P1</t>
   </si>
   <si>
-    <t>Out Ed A Adam</t>
-  </si>
-  <si>
-    <t>Phys Ed C Vero</t>
-  </si>
-  <si>
-    <t>Phys Ed A Adam</t>
-  </si>
-  <si>
-    <t>Phys Ed WOTP AM Vero</t>
-  </si>
-  <si>
-    <t>Phys Ed NV Vero</t>
-  </si>
-  <si>
-    <t>Out Ed B Chantal</t>
-  </si>
-  <si>
-    <t>Phys Ed D Adam</t>
-  </si>
-  <si>
-    <t>Phys Ed B Vero</t>
-  </si>
-  <si>
-    <t>Work1 WOTP PM Pam&amp;Keeley</t>
-  </si>
-  <si>
-    <t>Music NV Mike</t>
-  </si>
-  <si>
-    <t>Math WOTP AM Desmond</t>
-  </si>
-  <si>
-    <t>CCQ NV Mike</t>
-  </si>
-  <si>
-    <t>CCQ JS Nick</t>
-  </si>
-  <si>
-    <t>Music JS Mike</t>
-  </si>
-  <si>
-    <t>English JS Mo</t>
-  </si>
-  <si>
-    <t>Math E Andrew L</t>
-  </si>
-  <si>
-    <t>English2 WOTP AM Teacher X</t>
-  </si>
-  <si>
-    <t>Science E Carole</t>
-  </si>
-  <si>
-    <t>French C Teacher Y</t>
-  </si>
-  <si>
-    <t>Science NV Mike</t>
-  </si>
-  <si>
-    <t>CCQ E Sylvie</t>
-  </si>
-  <si>
-    <t>English G Cindy</t>
-  </si>
-  <si>
-    <t>Science A Teacher X</t>
-  </si>
-  <si>
-    <t>Tech G Andrew</t>
-  </si>
-  <si>
-    <t>History E Annie</t>
-  </si>
-  <si>
-    <t>French NV Caroline</t>
-  </si>
-  <si>
-    <t>French F Chantal</t>
-  </si>
-  <si>
-    <t>English B Cindy</t>
-  </si>
-  <si>
-    <t>Science G Carole</t>
-  </si>
-  <si>
-    <t>English C Mo</t>
-  </si>
-  <si>
-    <t>History JS Caroline</t>
-  </si>
-  <si>
-    <t>Tech F Andrew</t>
-  </si>
-  <si>
-    <t>Math A Andrew L</t>
-  </si>
-  <si>
-    <t>History D Annie</t>
-  </si>
-  <si>
-    <t>Science F Carole</t>
-  </si>
-  <si>
-    <t>History B Annie</t>
-  </si>
-  <si>
-    <t>CW D Sylvie</t>
-  </si>
-  <si>
-    <t>History C Annie</t>
-  </si>
-  <si>
-    <t>Science D Carole</t>
-  </si>
-  <si>
-    <t>CCQ D Sylvie</t>
-  </si>
-  <si>
-    <t>Math F Andrew</t>
-  </si>
-  <si>
-    <t>French D Teacher Y</t>
-  </si>
-  <si>
-    <t>Tech D Andrew</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>French G Chantal</t>
-  </si>
-  <si>
-    <t>English E Cindy</t>
-  </si>
-  <si>
-    <t>History A Teacher Y</t>
+    <t>A Out Ed Adam</t>
+  </si>
+  <si>
+    <t>B Out Ed Chantal</t>
+  </si>
+  <si>
+    <t>C History Annie</t>
+  </si>
+  <si>
+    <t>A English Mo</t>
+  </si>
+  <si>
+    <t>D French Teacher Y</t>
+  </si>
+  <si>
+    <t>B History Annie</t>
+  </si>
+  <si>
+    <t>E Math Andrew L</t>
+  </si>
+  <si>
+    <t>C Phys Ed Vero</t>
+  </si>
+  <si>
+    <t>F Science Carole</t>
+  </si>
+  <si>
+    <t>D Phys Ed Adam</t>
+  </si>
+  <si>
+    <t>F Tech Andrew</t>
+  </si>
+  <si>
+    <t>E Science Carole</t>
+  </si>
+  <si>
+    <t>G Science Carole</t>
+  </si>
+  <si>
+    <t>F English Cindy</t>
+  </si>
+  <si>
+    <t>G Tech Andrew</t>
+  </si>
+  <si>
+    <t>G Math Andrew</t>
+  </si>
+  <si>
+    <t>JS English Mo</t>
+  </si>
+  <si>
+    <t>JS CCQ Nick</t>
+  </si>
+  <si>
+    <t>A Phys Ed Adam</t>
+  </si>
+  <si>
+    <t>NV CCQ Nick</t>
+  </si>
+  <si>
+    <t>NV Science Mike</t>
+  </si>
+  <si>
+    <t>B Phys Ed Vero</t>
+  </si>
+  <si>
+    <t>NV Music Nick</t>
+  </si>
+  <si>
+    <t>WOTP AM Math Desmond</t>
+  </si>
+  <si>
+    <t>WOTP AM English Teacher X</t>
+  </si>
+  <si>
+    <t>JS Music Nick</t>
+  </si>
+  <si>
+    <t>WOTP AM Phys Ed Vero</t>
+  </si>
+  <si>
+    <t>NV Phys Ed Vero</t>
+  </si>
+  <si>
+    <t>WOTP PM Work1 Pam&amp;Keeley</t>
   </si>
   <si>
     <t>P2</t>
   </si>
   <si>
-    <t>Out Ed C Chantal</t>
-  </si>
-  <si>
-    <t>Out Ed Ex A Adam</t>
-  </si>
-  <si>
-    <t>Out Ed Ex C Chantal</t>
-  </si>
-  <si>
-    <t>Out Ed Ex E Adam</t>
-  </si>
-  <si>
-    <t>Phys Ed JS Vero</t>
-  </si>
-  <si>
-    <t>Out Ed D Adam</t>
-  </si>
-  <si>
-    <t>Out Ed Ex B Chantal</t>
-  </si>
-  <si>
-    <t>Out Ed Ex D Adam</t>
-  </si>
-  <si>
-    <t>Out Ed Ex F Chantal</t>
-  </si>
-  <si>
-    <t>Work2 WOTP PM Pam&amp;Keeley</t>
-  </si>
-  <si>
-    <t>CCQ Sc4Girls D Sylvie</t>
-  </si>
-  <si>
-    <t>Out Ed Ex G Chantal</t>
-  </si>
-  <si>
-    <t>French WOTP AM Caroline</t>
-  </si>
-  <si>
-    <t>Art E Desmond</t>
-  </si>
-  <si>
-    <t>English WOTP AM Teacher X</t>
-  </si>
-  <si>
-    <t>Music G Mike</t>
-  </si>
-  <si>
-    <t>CW F Mo</t>
-  </si>
-  <si>
-    <t>French E Vero</t>
-  </si>
-  <si>
-    <t>Math NV Desmond</t>
-  </si>
-  <si>
-    <t>Music F Mike</t>
-  </si>
-  <si>
-    <t>CW G Mo</t>
-  </si>
-  <si>
-    <t>History F Annie</t>
-  </si>
-  <si>
-    <t>French JS Caroline</t>
-  </si>
-  <si>
-    <t>English NV Mo</t>
-  </si>
-  <si>
-    <t>History G Annie</t>
-  </si>
-  <si>
-    <t>CCQ C Sylvie</t>
-  </si>
-  <si>
-    <t>Science B Carole</t>
-  </si>
-  <si>
-    <t>English D Cindy</t>
-  </si>
-  <si>
-    <t>CCQ F Sylvie</t>
-  </si>
-  <si>
-    <t>Math C Andrew L</t>
-  </si>
-  <si>
-    <t>CCQ A Teacher Y</t>
-  </si>
-  <si>
-    <t>Math JS Andrew L</t>
-  </si>
-  <si>
-    <t>Math G Andrew</t>
-  </si>
-  <si>
-    <t>French B Teacher Y</t>
-  </si>
-  <si>
-    <t>Math D Andrew</t>
+    <t>A Out Ed Ex Adam</t>
+  </si>
+  <si>
+    <t>B Out Ed Ex Chantal</t>
+  </si>
+  <si>
+    <t>B Science Carole</t>
+  </si>
+  <si>
+    <t>C Math Andrew L</t>
+  </si>
+  <si>
+    <t>C Out Ed Chantal</t>
+  </si>
+  <si>
+    <t>D English Cindy</t>
+  </si>
+  <si>
+    <t>D CCQ Sc4Girls Sylvie</t>
+  </si>
+  <si>
+    <t>E History Annie</t>
+  </si>
+  <si>
+    <t>D Out Ed Adam</t>
+  </si>
+  <si>
+    <t>E Out Ed Ex Adam</t>
+  </si>
+  <si>
+    <t>JS Science Mike</t>
+  </si>
+  <si>
+    <t>C Out Ed Ex Chantal</t>
+  </si>
+  <si>
+    <t>F Out Ed Ex Chantal</t>
+  </si>
+  <si>
+    <t>NV History Caroline</t>
+  </si>
+  <si>
+    <t>D Out Ed Ex Adam</t>
+  </si>
+  <si>
+    <t>G Out Ed Ex Chantal</t>
+  </si>
+  <si>
+    <t>JS Phys Ed Vero</t>
+  </si>
+  <si>
+    <t>WOTP PM Work2 Pam&amp;Keeley</t>
   </si>
   <si>
     <t>P3</t>
   </si>
   <si>
-    <t>Out Ed E Adam</t>
-  </si>
-  <si>
-    <t>Out Ed NV Adam</t>
-  </si>
-  <si>
-    <t>Out Ed F Chantal</t>
-  </si>
-  <si>
-    <t>Out Ed G Chantal</t>
-  </si>
-  <si>
-    <t>CCQ Sc4Boys F Sylvie</t>
-  </si>
-  <si>
-    <t>Work3 WOTP PM Pam&amp;Keeley</t>
-  </si>
-  <si>
-    <t>CCQ Sc4Boys G Sylvie</t>
-  </si>
-  <si>
-    <t>English WOTP PM Teacher X</t>
-  </si>
-  <si>
-    <t>Job Market WOTP AM Teacher X</t>
-  </si>
-  <si>
-    <t>English A Mo</t>
-  </si>
-  <si>
-    <t>French A Teacher Y</t>
-  </si>
-  <si>
-    <t>Math WOTP PM Desmond</t>
-  </si>
-  <si>
-    <t>English F Cindy</t>
-  </si>
-  <si>
-    <t>Art NV Desmond</t>
-  </si>
-  <si>
-    <t>Science C Carole</t>
-  </si>
-  <si>
-    <t>Science JS Mike</t>
-  </si>
-  <si>
-    <t>English2 WOTP PM Teacher X</t>
-  </si>
-  <si>
-    <t>Math B Andrew L</t>
+    <t>A French Teacher Y</t>
+  </si>
+  <si>
+    <t>C English Mo</t>
+  </si>
+  <si>
+    <t>C French Teacher Y</t>
+  </si>
+  <si>
+    <t>D Tech Andrew</t>
+  </si>
+  <si>
+    <t>D Science Carole</t>
+  </si>
+  <si>
+    <t>E Out Ed Adam</t>
+  </si>
+  <si>
+    <t>F CCQ Sc4Boys Sylvie</t>
+  </si>
+  <si>
+    <t>F History Annie</t>
+  </si>
+  <si>
+    <t>F Out Ed Chantal</t>
+  </si>
+  <si>
+    <t>F CW Mo</t>
+  </si>
+  <si>
+    <t>G CCQ Sc4Boys Sylvie</t>
+  </si>
+  <si>
+    <t>G CW Mo</t>
+  </si>
+  <si>
+    <t>G Out Ed Chantal</t>
+  </si>
+  <si>
+    <t>G History Annie</t>
+  </si>
+  <si>
+    <t>JS Math Andrew L</t>
+  </si>
+  <si>
+    <t>JS French Caroline</t>
+  </si>
+  <si>
+    <t>NV Math Desmond</t>
+  </si>
+  <si>
+    <t>NV Out Ed Adam</t>
+  </si>
+  <si>
+    <t>WOTP AM French Caroline</t>
+  </si>
+  <si>
+    <t>WOTP AM Job Market Teacher X</t>
+  </si>
+  <si>
+    <t>WOTP PM English Teacher X</t>
+  </si>
+  <si>
+    <t>WOTP PM Work3 Pam&amp;Keeley</t>
   </si>
   <si>
     <t>P4</t>
   </si>
   <si>
-    <t>Phys Ed E Adam</t>
-  </si>
-  <si>
-    <t>Work3 WOTP AM Pam&amp;Keeley</t>
-  </si>
-  <si>
-    <t>Phys Ed F Vero</t>
-  </si>
-  <si>
-    <t>Phys Ed G Vero</t>
-  </si>
-  <si>
-    <t>CCQ G Sylvie</t>
-  </si>
-  <si>
-    <t>French WOTP PM Caroline</t>
-  </si>
-  <si>
-    <t>History NV Caroline</t>
-  </si>
-  <si>
-    <t>CCQ B Sylvie</t>
-  </si>
-  <si>
-    <t>Art JS Desmond</t>
+    <t>A Science Teacher X</t>
+  </si>
+  <si>
+    <t>B English Cindy</t>
+  </si>
+  <si>
+    <t>B Math Andrew L</t>
+  </si>
+  <si>
+    <t>C Science Carole</t>
+  </si>
+  <si>
+    <t>D CW Sylvie</t>
+  </si>
+  <si>
+    <t>D History Annie</t>
+  </si>
+  <si>
+    <t>E Phys Ed Adam</t>
+  </si>
+  <si>
+    <t>F Math Andrew</t>
+  </si>
+  <si>
+    <t>F Phys Ed Vero</t>
+  </si>
+  <si>
+    <t>G French Chantal</t>
+  </si>
+  <si>
+    <t>G Phys Ed Vero</t>
+  </si>
+  <si>
+    <t>JS History Caroline</t>
+  </si>
+  <si>
+    <t>NV English Mo</t>
+  </si>
+  <si>
+    <t>WOTP AM Work3 Pam&amp;Keeley</t>
+  </si>
+  <si>
+    <t>WOTP AM English2 Teacher X</t>
+  </si>
+  <si>
+    <t>WOTP PM Math Desmond</t>
   </si>
   <si>
     <t>P5</t>
   </si>
   <si>
-    <t>Out Ed JS Vero</t>
-  </si>
-  <si>
-    <t>Phys Ed WOTP PM Vero</t>
-  </si>
-  <si>
-    <t>Work2 WOTP AM Pam&amp;Keeley</t>
-  </si>
-  <si>
-    <t>Art C Desmond</t>
-  </si>
-  <si>
-    <t>Job Market WOTP PM Teacher X</t>
-  </si>
-  <si>
-    <t>Music D Mike</t>
-  </si>
-  <si>
-    <t>Music B Mike</t>
-  </si>
-  <si>
-    <t>Art A Desmond</t>
+    <t>A History Teacher Y</t>
+  </si>
+  <si>
+    <t>D Math Andrew</t>
+  </si>
+  <si>
+    <t>E English Cindy</t>
+  </si>
+  <si>
+    <t>JS Out Ed Vero</t>
+  </si>
+  <si>
+    <t>NV French Caroline</t>
+  </si>
+  <si>
+    <t>WOTP AM Work2 Pam&amp;Keeley</t>
+  </si>
+  <si>
+    <t>WOTP PM Phys Ed Vero</t>
+  </si>
+  <si>
+    <t>WOTP PM French Caroline</t>
   </si>
   <si>
     <t>P6</t>
   </si>
   <si>
-    <t>Work1 WOTP AM Pam&amp;Keeley</t>
+    <t>A Math Andrew L</t>
+  </si>
+  <si>
+    <t>B French Teacher Y</t>
+  </si>
+  <si>
+    <t>C Art Desmond</t>
+  </si>
+  <si>
+    <t>D Music Mike</t>
+  </si>
+  <si>
+    <t>E French Vero</t>
+  </si>
+  <si>
+    <t>E Art Desmond</t>
+  </si>
+  <si>
+    <t>F French Chantal</t>
+  </si>
+  <si>
+    <t>F Music Mike</t>
+  </si>
+  <si>
+    <t>G English Cindy</t>
+  </si>
+  <si>
+    <t>G Music Mike</t>
+  </si>
+  <si>
+    <t>WOTP AM Work1 Pam&amp;Keeley</t>
+  </si>
+  <si>
+    <t>WOTP PM Job Market Teacher X</t>
   </si>
 </sst>
 </file>
@@ -579,340 +543,340 @@
         <v>7</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="F3" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2"/>
       <c r="C4" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="F4" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2"/>
       <c r="C5" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="G5" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2"/>
       <c r="C6" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="F6" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="G6" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2"/>
       <c r="C7" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="F7" s="5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="G7" s="5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2"/>
       <c r="C8" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="F8" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="G8" s="5" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2"/>
       <c r="C9" s="5" t="s">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="E9" s="5" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="F9" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2"/>
       <c r="C10" s="5" t="s">
-        <v>35</v>
+        <v>9</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="E10" s="5" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>25</v>
+        <v>7</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2"/>
       <c r="C11" s="5" t="s">
-        <v>38</v>
+        <v>10</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="E11" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="F11" s="5" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="G11" s="5" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="2"/>
       <c r="C12" s="5" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>41</v>
+        <v>13</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="F12" s="5" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
       <c r="G12" s="5" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="2"/>
       <c r="C13" s="5" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="E13" s="5" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="F13" s="5" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
       <c r="G13" s="5" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="2"/>
       <c r="C14" s="5" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="E14" s="5" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="F14" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="2"/>
       <c r="C15" s="5" t="s">
-        <v>52</v>
+        <v>18</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>53</v>
+        <v>19</v>
       </c>
       <c r="E15" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F15" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="2"/>
       <c r="C16" s="5" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>50</v>
+        <v>21</v>
       </c>
       <c r="E16" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F16" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G16" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="2"/>
       <c r="C17" s="5" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D17" s="5" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F17" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="2"/>
       <c r="C18" s="5" t="s">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="E18" s="5" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="F18" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G18" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="2"/>
       <c r="C19" s="5" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>50</v>
+        <v>28</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="F19" s="5" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="2"/>
       <c r="C20" s="5" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="F20" s="5" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
       <c r="G20" s="5" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="3"/>
       <c r="C21" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="E21" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>50</v>
+        <v>36</v>
       </c>
     </row>
     <row r="22">
@@ -924,346 +888,346 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="s">
-        <v>54</v>
+        <v>37</v>
       </c>
       <c r="C23" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
       <c r="D23" s="5" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="E23" s="5" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="F23" s="5" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="2"/>
       <c r="C24" s="5" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="E24" s="5" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="F24" s="5" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="G24" s="5" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="2"/>
       <c r="C25" s="5" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="E25" s="5" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="F25" s="5" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" s="2"/>
       <c r="C26" s="5" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="E26" s="5" t="s">
-        <v>16</v>
+        <v>7</v>
       </c>
       <c r="F26" s="5" t="s">
-        <v>64</v>
+        <v>7</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="2"/>
       <c r="C27" s="5" t="s">
-        <v>19</v>
+        <v>7</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="E27" s="5" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="F27" s="5" t="s">
-        <v>20</v>
+        <v>7</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" s="2"/>
       <c r="C28" s="5" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="F28" s="5" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="G28" s="5" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="2"/>
       <c r="C29" s="5" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>76</v>
+        <v>38</v>
       </c>
       <c r="E29" s="5" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="F29" s="5" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="2"/>
       <c r="C30" s="5" t="s">
-        <v>79</v>
+        <v>11</v>
       </c>
       <c r="D30" s="5" t="s">
-        <v>75</v>
+        <v>39</v>
       </c>
       <c r="E30" s="5" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
       <c r="F30" s="5" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
       <c r="G30" s="5" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="2"/>
       <c r="C31" s="5" t="s">
-        <v>71</v>
+        <v>40</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>79</v>
+        <v>41</v>
       </c>
       <c r="E31" s="5" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="F31" s="5" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" s="2"/>
       <c r="C32" s="5" t="s">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>25</v>
+        <v>43</v>
       </c>
       <c r="E32" s="5" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="F32" s="5" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="G32" s="5" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" s="2"/>
       <c r="C33" s="5" t="s">
-        <v>24</v>
+        <v>44</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>86</v>
+        <v>45</v>
       </c>
       <c r="E33" s="5" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="F33" s="5" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="2"/>
       <c r="C34" s="5" t="s">
-        <v>88</v>
+        <v>46</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E34" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F34" s="5" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="G34" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="2"/>
       <c r="C35" s="5" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>89</v>
+        <v>16</v>
       </c>
       <c r="E35" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F35" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" s="2"/>
       <c r="C36" s="5" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="E36" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F36" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G36" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="2"/>
       <c r="C37" s="5" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E37" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F37" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G37" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="2"/>
       <c r="C38" s="5" t="s">
-        <v>50</v>
+        <v>25</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="E38" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F38" s="5" t="s">
         <v>50</v>
       </c>
       <c r="G38" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="2"/>
       <c r="C39" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="E39" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F39" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G39" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="2"/>
       <c r="C40" s="5" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="E40" s="5" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="F40" s="5" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="G40" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="3"/>
       <c r="C41" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D41" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="E41" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="F41" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="G41" s="5" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
     </row>
     <row r="42">
@@ -1275,346 +1239,346 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="s">
-        <v>90</v>
+        <v>56</v>
       </c>
       <c r="C43" s="5" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="E43" s="5" t="s">
-        <v>92</v>
+        <v>7</v>
       </c>
       <c r="F43" s="5" t="s">
-        <v>58</v>
+        <v>7</v>
       </c>
       <c r="G43" s="5" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" s="2"/>
       <c r="C44" s="5" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>56</v>
+        <v>7</v>
       </c>
       <c r="E44" s="5" t="s">
-        <v>57</v>
+        <v>7</v>
       </c>
       <c r="F44" s="5" t="s">
-        <v>63</v>
+        <v>7</v>
       </c>
       <c r="G44" s="5" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" s="2"/>
       <c r="C45" s="5" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="E45" s="5" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="F45" s="5" t="s">
-        <v>66</v>
+        <v>7</v>
       </c>
       <c r="G45" s="5" t="s">
-        <v>46</v>
+        <v>7</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" s="2"/>
       <c r="C46" s="5" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
       <c r="D46" s="5" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="E46" s="5" t="s">
-        <v>17</v>
+        <v>7</v>
       </c>
       <c r="F46" s="5" t="s">
-        <v>96</v>
+        <v>7</v>
       </c>
       <c r="G46" s="5" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" s="2"/>
       <c r="C47" s="5" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>67</v>
+        <v>7</v>
       </c>
       <c r="E47" s="5" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>69</v>
+        <v>7</v>
       </c>
       <c r="G47" s="5" t="s">
-        <v>42</v>
+        <v>7</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" s="2"/>
       <c r="C48" s="5" t="s">
-        <v>99</v>
+        <v>57</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
       <c r="E48" s="5" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
       <c r="G48" s="5" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" s="2"/>
       <c r="C49" s="5" t="s">
-        <v>102</v>
+        <v>13</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>103</v>
+        <v>39</v>
       </c>
       <c r="E49" s="5" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="G49" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="2"/>
       <c r="C50" s="5" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>87</v>
+        <v>59</v>
       </c>
       <c r="E50" s="5" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="F50" s="5" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
       <c r="G50" s="5" t="s">
-        <v>101</v>
+        <v>7</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" s="2"/>
       <c r="C51" s="5" t="s">
-        <v>101</v>
+        <v>60</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="E51" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="F51" s="5" t="s">
-        <v>105</v>
+        <v>7</v>
       </c>
       <c r="G51" s="5" t="s">
-        <v>104</v>
+        <v>7</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" s="2"/>
       <c r="C52" s="5" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>105</v>
+        <v>61</v>
       </c>
       <c r="E52" s="5" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="F52" s="5" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
       <c r="G52" s="5" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" s="2"/>
       <c r="C53" s="5" t="s">
-        <v>89</v>
+        <v>62</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="E53" s="5" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="G53" s="5" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" s="2"/>
       <c r="C54" s="5" t="s">
-        <v>42</v>
+        <v>63</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="E54" s="5" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G54" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" s="2"/>
       <c r="C55" s="5" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="D55" s="5" t="s">
-        <v>50</v>
+        <v>66</v>
       </c>
       <c r="E55" s="5" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G55" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" s="2"/>
       <c r="C56" s="5" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="E56" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G56" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" s="2"/>
       <c r="C57" s="5" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="E57" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G57" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" s="2"/>
       <c r="C58" s="5" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="D58" s="5" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="E58" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="G58" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" s="2"/>
       <c r="C59" s="5" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="E59" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F59" s="5" t="s">
         <v>50</v>
       </c>
       <c r="G59" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" s="2"/>
       <c r="C60" s="5" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>50</v>
+        <v>76</v>
       </c>
       <c r="E60" s="5" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G60" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" s="3"/>
       <c r="C61" s="5" t="s">
-        <v>50</v>
+        <v>77</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="E61" s="5" t="s">
-        <v>50</v>
+        <v>74</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>50</v>
+        <v>78</v>
       </c>
       <c r="G61" s="5" t="s">
-        <v>50</v>
+        <v>34</v>
       </c>
     </row>
     <row r="62">
@@ -1626,19 +1590,19 @@
     </row>
     <row r="63">
       <c r="A63" s="1" t="s">
-        <v>109</v>
+        <v>79</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="E63" s="5" t="s">
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="G63" s="5" t="s">
         <v>7</v>
@@ -1647,325 +1611,325 @@
     <row r="64">
       <c r="A64" s="2"/>
       <c r="C64" s="5" t="s">
-        <v>111</v>
+        <v>7</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="E64" s="5" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="G64" s="5" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" s="2"/>
       <c r="C65" s="5" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="E65" s="5" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="G65" s="5" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" s="2"/>
       <c r="C66" s="5" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>99</v>
+        <v>7</v>
       </c>
       <c r="E66" s="5" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="G66" s="5" t="s">
-        <v>115</v>
+        <v>7</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" s="2"/>
       <c r="C67" s="5" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="E67" s="5" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="G67" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="2"/>
       <c r="C68" s="5" t="s">
-        <v>81</v>
+        <v>7</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="E68" s="5" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>44</v>
+        <v>7</v>
       </c>
       <c r="G68" s="5" t="s">
-        <v>105</v>
+        <v>7</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" s="2"/>
       <c r="C69" s="5" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="E69" s="5" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="G69" s="5" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" s="2"/>
       <c r="C70" s="5" t="s">
-        <v>31</v>
+        <v>80</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
       <c r="E70" s="5" t="s">
-        <v>29</v>
+        <v>7</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="G70" s="5" t="s">
-        <v>89</v>
+        <v>7</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" s="2"/>
       <c r="C71" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D71" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="D71" s="5" t="s">
-        <v>101</v>
-      </c>
       <c r="E71" s="5" t="s">
-        <v>102</v>
+        <v>7</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="G71" s="5" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="2"/>
       <c r="C72" s="5" t="s">
-        <v>47</v>
+        <v>59</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="E72" s="5" t="s">
-        <v>26</v>
+        <v>7</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>30</v>
+        <v>7</v>
       </c>
       <c r="G72" s="5" t="s">
-        <v>83</v>
+        <v>7</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" s="2"/>
       <c r="C73" s="5" t="s">
-        <v>51</v>
+        <v>84</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="E73" s="5" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>38</v>
+        <v>7</v>
       </c>
       <c r="G73" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" s="2"/>
       <c r="C74" s="5" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>50</v>
+        <v>85</v>
       </c>
       <c r="E74" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>41</v>
+        <v>7</v>
       </c>
       <c r="G74" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="2"/>
       <c r="C75" s="5" t="s">
-        <v>50</v>
+        <v>19</v>
       </c>
       <c r="D75" s="5" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="E75" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>48</v>
+        <v>7</v>
       </c>
       <c r="G75" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="2"/>
       <c r="C76" s="5" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="E76" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G76" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="2"/>
       <c r="C77" s="5" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="E77" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G77" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="2"/>
       <c r="C78" s="5" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="E78" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G78" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="2"/>
       <c r="C79" s="5" t="s">
-        <v>50</v>
+        <v>35</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="E79" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G79" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" s="2"/>
       <c r="C80" s="5" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="D80" s="5" t="s">
-        <v>50</v>
+        <v>94</v>
       </c>
       <c r="E80" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G80" s="5" t="s">
-        <v>50</v>
+        <v>8</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="3"/>
       <c r="C81" s="5" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>50</v>
+        <v>95</v>
       </c>
       <c r="E81" s="5" t="s">
-        <v>50</v>
+        <v>93</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G81" s="5" t="s">
-        <v>50</v>
+        <v>9</v>
       </c>
     </row>
     <row r="82">
@@ -1977,346 +1941,346 @@
     </row>
     <row r="83">
       <c r="A83" s="1" t="s">
-        <v>119</v>
+        <v>96</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>120</v>
+        <v>7</v>
       </c>
       <c r="E83" s="5" t="s">
-        <v>59</v>
+        <v>7</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G83" s="5" t="s">
-        <v>55</v>
+        <v>7</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" s="2"/>
       <c r="C84" s="5" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="E84" s="5" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="F84" s="5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="G84" s="5" t="s">
-        <v>60</v>
+        <v>7</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" s="2"/>
       <c r="C85" s="5" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>52</v>
+        <v>7</v>
       </c>
       <c r="E85" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="F85" s="5" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
       <c r="G85" s="5" t="s">
-        <v>65</v>
+        <v>7</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="2"/>
       <c r="C86" s="5" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="D86" s="5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="E86" s="5" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>124</v>
+        <v>7</v>
       </c>
       <c r="G86" s="5" t="s">
-        <v>122</v>
+        <v>7</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" s="2"/>
       <c r="C87" s="5" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="D87" s="5" t="s">
-        <v>47</v>
+        <v>7</v>
       </c>
       <c r="E87" s="5" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
       <c r="G87" s="5" t="s">
-        <v>24</v>
+        <v>7</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" s="2"/>
       <c r="C88" s="5" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="D88" s="5" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="E88" s="5" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="G88" s="5" t="s">
-        <v>124</v>
+        <v>7</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" s="2"/>
       <c r="C89" s="5" t="s">
-        <v>126</v>
+        <v>97</v>
       </c>
       <c r="D89" s="5" t="s">
-        <v>40</v>
+        <v>7</v>
       </c>
       <c r="E89" s="5" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="G89" s="5" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" s="2"/>
       <c r="C90" s="5" t="s">
-        <v>127</v>
+        <v>82</v>
       </c>
       <c r="D90" s="5" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="E90" s="5" t="s">
-        <v>51</v>
+        <v>7</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>114</v>
+        <v>7</v>
       </c>
       <c r="G90" s="5" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" s="2"/>
       <c r="C91" s="5" t="s">
-        <v>116</v>
+        <v>83</v>
       </c>
       <c r="D91" s="5" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="E91" s="5" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>103</v>
+        <v>7</v>
       </c>
       <c r="G91" s="5" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" s="2"/>
       <c r="C92" s="5" t="s">
-        <v>25</v>
+        <v>98</v>
       </c>
       <c r="D92" s="5" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="E92" s="5" t="s">
-        <v>117</v>
+        <v>7</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="G92" s="5" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" s="2"/>
       <c r="C93" s="5" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="D93" s="5" t="s">
-        <v>115</v>
+        <v>58</v>
       </c>
       <c r="E93" s="5" t="s">
-        <v>124</v>
+        <v>7</v>
       </c>
       <c r="F93" s="5" t="s">
-        <v>49</v>
+        <v>7</v>
       </c>
       <c r="G93" s="5" t="s">
-        <v>77</v>
+        <v>7</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="2"/>
       <c r="C94" s="5" t="s">
-        <v>43</v>
+        <v>66</v>
       </c>
       <c r="D94" s="5" t="s">
-        <v>73</v>
+        <v>12</v>
       </c>
       <c r="E94" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F94" s="5" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="G94" s="5" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" s="2"/>
       <c r="C95" s="5" t="s">
-        <v>50</v>
+        <v>64</v>
       </c>
       <c r="D95" s="5" t="s">
-        <v>50</v>
+        <v>99</v>
       </c>
       <c r="E95" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F95" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G95" s="5" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" s="2"/>
       <c r="C96" s="5" t="s">
-        <v>50</v>
+        <v>70</v>
       </c>
       <c r="D96" s="5" t="s">
-        <v>50</v>
+        <v>87</v>
       </c>
       <c r="E96" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F96" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G96" s="5" t="s">
-        <v>53</v>
+        <v>7</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" s="2"/>
       <c r="C97" s="5" t="s">
-        <v>50</v>
+        <v>68</v>
       </c>
       <c r="D97" s="5" t="s">
-        <v>50</v>
+        <v>89</v>
       </c>
       <c r="E97" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G97" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" s="2"/>
       <c r="C98" s="5" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="D98" s="5" t="s">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="E98" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G98" s="5" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" s="2"/>
       <c r="C99" s="5" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="D99" s="5" t="s">
-        <v>50</v>
+        <v>73</v>
       </c>
       <c r="E99" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F99" s="5" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="G99" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" s="2"/>
       <c r="C100" s="5" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="D100" s="5" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="E100" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="G100" s="5" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" s="3"/>
       <c r="C101" s="5" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="D101" s="5" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="E101" s="5" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
       <c r="G101" s="5" t="s">
-        <v>50</v>
+        <v>102</v>
       </c>
     </row>
     <row r="102">
@@ -2328,346 +2292,346 @@
     </row>
     <row r="103">
       <c r="A103" s="1" t="s">
-        <v>128</v>
+        <v>105</v>
       </c>
       <c r="C103" s="5" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="D103" s="5" t="s">
-        <v>121</v>
+        <v>7</v>
       </c>
       <c r="E103" s="5" t="s">
-        <v>110</v>
+        <v>7</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G103" s="5" t="s">
-        <v>91</v>
+        <v>7</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" s="2"/>
       <c r="C104" s="5" t="s">
-        <v>28</v>
+        <v>7</v>
       </c>
       <c r="D104" s="5" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="E104" s="5" t="s">
-        <v>112</v>
+        <v>7</v>
       </c>
       <c r="F104" s="5" t="s">
-        <v>13</v>
+        <v>7</v>
       </c>
       <c r="G104" s="5" t="s">
-        <v>93</v>
+        <v>7</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" s="2"/>
       <c r="C105" s="5" t="s">
-        <v>108</v>
+        <v>7</v>
       </c>
       <c r="D105" s="5" t="s">
-        <v>68</v>
+        <v>7</v>
       </c>
       <c r="E105" s="5" t="s">
-        <v>113</v>
+        <v>7</v>
       </c>
       <c r="F105" s="5" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="G105" s="5" t="s">
-        <v>94</v>
+        <v>7</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="2"/>
       <c r="C106" s="5" t="s">
-        <v>72</v>
+        <v>7</v>
       </c>
       <c r="D106" s="5" t="s">
-        <v>74</v>
+        <v>7</v>
       </c>
       <c r="E106" s="5" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
       <c r="F106" s="5" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
       <c r="G106" s="5" t="s">
-        <v>95</v>
+        <v>7</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" s="2"/>
       <c r="C107" s="5" t="s">
-        <v>106</v>
+        <v>7</v>
       </c>
       <c r="D107" s="5" t="s">
-        <v>70</v>
+        <v>7</v>
       </c>
       <c r="E107" s="5" t="s">
-        <v>107</v>
+        <v>7</v>
       </c>
       <c r="F107" s="5" t="s">
-        <v>127</v>
+        <v>7</v>
       </c>
       <c r="G107" s="5" t="s">
-        <v>97</v>
+        <v>7</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" s="2"/>
       <c r="C108" s="5" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D108" s="5" t="s">
-        <v>84</v>
+        <v>7</v>
       </c>
       <c r="E108" s="5" t="s">
-        <v>80</v>
+        <v>7</v>
       </c>
       <c r="F108" s="5" t="s">
-        <v>126</v>
+        <v>7</v>
       </c>
       <c r="G108" s="5" t="s">
-        <v>129</v>
+        <v>7</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" s="2"/>
       <c r="C109" s="5" t="s">
-        <v>36</v>
+        <v>7</v>
       </c>
       <c r="D109" s="5" t="s">
-        <v>78</v>
+        <v>7</v>
       </c>
       <c r="E109" s="5" t="s">
-        <v>82</v>
+        <v>7</v>
       </c>
       <c r="F109" s="5" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="G109" s="5" t="s">
-        <v>125</v>
+        <v>7</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" s="2"/>
       <c r="C110" s="5" t="s">
-        <v>73</v>
+        <v>7</v>
       </c>
       <c r="D110" s="5" t="s">
-        <v>37</v>
+        <v>7</v>
       </c>
       <c r="E110" s="5" t="s">
-        <v>88</v>
+        <v>7</v>
       </c>
       <c r="F110" s="5" t="s">
-        <v>86</v>
+        <v>7</v>
       </c>
       <c r="G110" s="5" t="s">
-        <v>123</v>
+        <v>7</v>
       </c>
     </row>
     <row r="111">
       <c r="A111" s="2"/>
       <c r="C111" s="5" t="s">
-        <v>49</v>
+        <v>106</v>
       </c>
       <c r="D111" s="5" t="s">
-        <v>53</v>
+        <v>97</v>
       </c>
       <c r="E111" s="5" t="s">
-        <v>100</v>
+        <v>7</v>
       </c>
       <c r="F111" s="5" t="s">
-        <v>27</v>
+        <v>7</v>
       </c>
       <c r="G111" s="5" t="s">
-        <v>88</v>
+        <v>7</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="2"/>
       <c r="C112" s="5" t="s">
-        <v>45</v>
+        <v>107</v>
       </c>
       <c r="D112" s="5" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="E112" s="5" t="s">
-        <v>118</v>
+        <v>7</v>
       </c>
       <c r="F112" s="5" t="s">
-        <v>71</v>
+        <v>7</v>
       </c>
       <c r="G112" s="5" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="2"/>
       <c r="C113" s="5" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="D113" s="5" t="s">
-        <v>45</v>
+        <v>10</v>
       </c>
       <c r="E113" s="5" t="s">
-        <v>32</v>
+        <v>7</v>
       </c>
       <c r="F113" s="5" t="s">
-        <v>76</v>
+        <v>7</v>
       </c>
       <c r="G113" s="5" t="s">
-        <v>98</v>
+        <v>7</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" s="2"/>
       <c r="C114" s="5" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D114" s="5" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="E114" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F114" s="5" t="s">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="G114" s="5" t="s">
-        <v>39</v>
+        <v>7</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" s="2"/>
       <c r="C115" s="5" t="s">
-        <v>50</v>
+        <v>110</v>
       </c>
       <c r="D115" s="5" t="s">
-        <v>50</v>
+        <v>111</v>
       </c>
       <c r="E115" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F115" s="5" t="s">
-        <v>75</v>
+        <v>7</v>
       </c>
       <c r="G115" s="5" t="s">
-        <v>116</v>
+        <v>7</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" s="2"/>
       <c r="C116" s="5" t="s">
-        <v>50</v>
+        <v>112</v>
       </c>
       <c r="D116" s="5" t="s">
-        <v>50</v>
+        <v>113</v>
       </c>
       <c r="E116" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F116" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G116" s="5" t="s">
-        <v>50</v>
+        <v>62</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" s="2"/>
       <c r="C117" s="5" t="s">
-        <v>50</v>
+        <v>114</v>
       </c>
       <c r="D117" s="5" t="s">
-        <v>50</v>
+        <v>115</v>
       </c>
       <c r="E117" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="F117" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G117" s="5" t="s">
-        <v>50</v>
+        <v>63</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" s="2"/>
       <c r="C118" s="5" t="s">
-        <v>50</v>
+        <v>72</v>
       </c>
       <c r="D118" s="5" t="s">
-        <v>50</v>
+        <v>71</v>
       </c>
       <c r="E118" s="5" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="F118" s="5" t="s">
-        <v>50</v>
+        <v>7</v>
       </c>
       <c r="G118" s="5" t="s">
-        <v>50</v>
+        <v>65</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" s="2"/>
       <c r="C119" s="5" t="s">
-        <v>50</v>
+        <v>92</v>
       </c>
       <c r="D119" s="5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="E119" s="5" t="s">
-        <v>50</v>
+        <v>88</v>
       </c>
       <c r="F119" s="5" t="s">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="G119" s="5" t="s">
-        <v>50</v>
+        <v>67</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" s="2"/>
       <c r="C120" s="5" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="D120" s="5" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="E120" s="5" t="s">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="F120" s="5" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="G120" s="5" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" s="3"/>
       <c r="C121" s="5" t="s">
-        <v>50</v>
+        <v>117</v>
       </c>
       <c r="D121" s="5" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="E121" s="5" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="F121" s="5" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
       <c r="G121" s="5" t="s">
-        <v>50</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>